<commit_message>
adding miles from data
</commit_message>
<xml_diff>
--- a/clean_drive_data.xlsx
+++ b/clean_drive_data.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="8" documentId="8_{C8644156-8E24-4051-966E-B875010AEA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E070D4ED-B66B-4AB8-BB74-80A926F0CAC9}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="720" windowWidth="16164" windowHeight="12240" xr2:uid="{D6BC6051-01A3-49F8-B82F-F77B1A5CE531}"/>
+    <workbookView xWindow="3384" yWindow="444" windowWidth="16164" windowHeight="12240" xr2:uid="{D6BC6051-01A3-49F8-B82F-F77B1A5CE531}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -879,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266353BA-17FB-46DF-8C70-166242BCD8FE}">
   <dimension ref="A1:L1376"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1354" workbookViewId="0">
-      <selection activeCell="A1299" sqref="A1299:L1372"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
cleaned data and made graph
</commit_message>
<xml_diff>
--- a/clean_drive_data.xlsx
+++ b/clean_drive_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ac46583d1abce789/Desktop/Simulation/ElectricTransitSim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{C8644156-8E24-4051-966E-B875010AEA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E070D4ED-B66B-4AB8-BB74-80A926F0CAC9}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{C8644156-8E24-4051-966E-B875010AEA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A1F7343-9270-4AF5-8CF4-2C6DBBC0B0E8}"/>
   <bookViews>
-    <workbookView xWindow="3384" yWindow="444" windowWidth="16164" windowHeight="12240" xr2:uid="{D6BC6051-01A3-49F8-B82F-F77B1A5CE531}"/>
+    <workbookView xWindow="3888" yWindow="816" windowWidth="16164" windowHeight="11424" xr2:uid="{D6BC6051-01A3-49F8-B82F-F77B1A5CE531}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -880,7 +880,7 @@
   <dimension ref="A1:L1376"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>